<commit_message>
Add value sets and update profile field descriptions/definitions
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-prat-encounter.xlsx
+++ b/output/StructureDefinition-prat-encounter.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3090" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3087" uniqueCount="497">
   <si>
     <t>Path</t>
   </si>
@@ -360,10 +360,7 @@
 </t>
   </si>
   <si>
-    <t>Identifier(s) by which this encounter is known</t>
-  </si>
-  <si>
-    <t>Identifier(s) by which this encounter is known.</t>
+    <t>Identifier(s) by which this timepoint is known</t>
   </si>
   <si>
     <t>Event.identifier</t>
@@ -577,19 +574,13 @@
     <t>Encounter.status</t>
   </si>
   <si>
-    <t>planned | arrived | triaged | in-progress | onleave | finished | cancelled +</t>
-  </si>
-  <si>
-    <t>planned | arrived | triaged | in-progress | onleave | finished | cancelled +.</t>
+    <t>in-progress | finished | planned</t>
   </si>
   <si>
     <t>Note that internal business rules will determine the appropriate transitions that may occur between statuses (and also classes).</t>
   </si>
   <si>
-    <t>Current state of the encounter.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/encounter-status|4.0.1</t>
+    <t>http://hl7.org/fhir/us/pacio-rat/ValueSet/prat-status-vs</t>
   </si>
   <si>
     <t>Event.status</t>
@@ -611,10 +602,10 @@
 </t>
   </si>
   <si>
-    <t>List of past encounter statuses</t>
-  </si>
-  <si>
-    <t>The status history permits the encounter resource to contain the status history without needing to read through the historical versions of the resource, or even have the server store them.</t>
+    <t>List of past timepoint statuses</t>
+  </si>
+  <si>
+    <t>The status history permits this resource to contain the status history without needing to read through the historical versions of the resource, or even have the server store them.</t>
   </si>
   <si>
     <t>The current status is always found in the current version of the resource, not the status history.</t>
@@ -662,10 +653,10 @@
 </t>
   </si>
   <si>
-    <t>Classification of patient encounter</t>
-  </si>
-  <si>
-    <t>Concepts representing classification of patient encounter such as ambulatory (outpatient), inpatient, emergency, home health or others due to local variations.</t>
+    <t>Classification of patient timepoint</t>
+  </si>
+  <si>
+    <t>Concepts representing classification of patient timepoint such as ambulatory (outpatient), inpatient, emergency, home health or others due to local variations.</t>
   </si>
   <si>
     <t>Classification of the encounter.</t>
@@ -686,10 +677,10 @@
     <t>Encounter.classHistory</t>
   </si>
   <si>
-    <t>List of past encounter classes</t>
-  </si>
-  <si>
-    <t>The class history permits the tracking of the encounters transitions without needing to go  through the resource history.  This would be used for a case where an admission starts of as an emergency encounter, then transitions into an inpatient scenario. Doing this and not restarting a new encounter ensures that any lab/diagnostic results can more easily follow the patient and not require re-processing and not get lost or cancelled during a kind of discharge from emergency to inpatient.</t>
+    <t>List of past timepoint classes</t>
+  </si>
+  <si>
+    <t>The class history permits the tracking of the timepoints transitions without needing to go through the resource history. This would be used for a case where an admission starts of as an emergency encounter, then transitions into an inpatient scenario. Doing this and not restarting a new timepoint ensures that any lab/diagnostic results can more easily follow the patient and not require re-processing and not get lost or cancelled during a kind of discharge from emergency to inpatient.</t>
   </si>
   <si>
     <t>Encounter.classHistory.id</t>
@@ -722,10 +713,6 @@
     <t>Encounter.type</t>
   </si>
   <si>
-    <t>Payer
-Regulatory - StateRegulatory - FederalProviderAccreditation Agency</t>
-  </si>
-  <si>
     <t>The entity structuring the timepoint</t>
   </si>
   <si>
@@ -735,10 +722,7 @@
     <t>Since there are many ways to further classify encounters, this element is 0..*.</t>
   </si>
   <si>
-    <t>Valueset to describe the Encounter Type</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/ValueSet/us-core-encounter-type</t>
+    <t>http://hl7.org/fhir/us/pacio-rat/ValueSet/prat-entity-type-vs</t>
   </si>
   <si>
     <t>Event.code</t>
@@ -774,7 +758,7 @@
     <t>Encounter.priority</t>
   </si>
   <si>
-    <t>Indicates the urgency of the encounter</t>
+    <t>Indicates the urgency of the timepoint</t>
   </si>
   <si>
     <t>Indicates the urgency of the encounter.</t>
@@ -803,10 +787,7 @@
 </t>
   </si>
   <si>
-    <t>The patient or group present at the encounter</t>
-  </si>
-  <si>
-    <t>The patient or group present at the encounter.</t>
+    <t>The patient present at the timepoint</t>
   </si>
   <si>
     <t>While the encounter is always about the patient, the patient might not actually be known in all contexts of use, and there may be a group of patients that could be anonymous (such as in a group therapy for Alcoholics Anonymous - where the recording of the encounter could be used for billing on the number of people/staff and not important to the context of the specific patients) or alternately in veterinary care a herd of sheep receiving treatment (where the animals are not individually tracked).</t>
@@ -831,10 +812,10 @@
 </t>
   </si>
   <si>
-    <t>Episode(s) of care that this encounter should be recorded against</t>
-  </si>
-  <si>
-    <t>Where a specific encounter should be classified as a part of a specific episode(s) of care this field should be used. This association can facilitate grouping of related encounters together for a specific purpose, such as government reporting, issue tracking, association via a common problem.  The association is recorded on the encounter as these are typically created after the episode of care and grouped on entry rather than editing the episode of care to append another encounter to it (the episode of care could span years).</t>
+    <t>Episode(s) of care that this timepoint should be recorded against</t>
+  </si>
+  <si>
+    <t>Where a specific timepoint should be classified as a part of a specific episode(s) of care this field should be used. This association can facilitate grouping of related timepoints together for a specific purpose, such as government reporting, issue tracking, association via a common problem. The association is recorded on the timepoint as these are typically created after the episode of care and grouped on entry rather than editing the episode of care to append another timepoint to it (the episode of care could span years).</t>
   </si>
   <si>
     <t>Event.context</t>
@@ -995,15 +976,18 @@
     <t>Encounter.participant.type</t>
   </si>
   <si>
-    <t>Role of participant in encounter</t>
+    <t>Role of participant in timepoint</t>
+  </si>
+  <si>
+    <t>Role of participant in timepoint.</t>
+  </si>
+  <si>
+    <t>The participant type indicates how an individual participates in an encounter. It includes non-practitioner participants, and for practitioners this is to describe the action type in the context of this encounter (e.g. Admitting Dr, Attending Dr, Translator, Consulting Dr). This is different to the practitioner roles which are functional roles, derived from terms of employment, education, licensing, etc.</t>
   </si>
   <si>
     <t>Role of participant in encounter.</t>
   </si>
   <si>
-    <t>The participant type indicates how an individual participates in an encounter. It includes non-practitioner participants, and for practitioners this is to describe the action type in the context of this encounter (e.g. Admitting Dr, Attending Dr, Translator, Consulting Dr). This is different to the practitioner roles which are functional roles, derived from terms of employment, education, licensing, etc.</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/ValueSet/encounter-participant-type</t>
   </si>
   <si>
@@ -1019,10 +1003,10 @@
     <t>Encounter.participant.period</t>
   </si>
   <si>
-    <t>Period of time during the encounter that the participant participated</t>
-  </si>
-  <si>
-    <t>The period of time that the specified participant participated in the encounter. These can overlap or be sub-sets of the overall encounter's period.</t>
+    <t>Period of time during the timepoint that the participant participated</t>
+  </si>
+  <si>
+    <t>The period of time that the specified participant participated in the timepoint. These can overlap or be sub-sets of the overall timepoint's period.</t>
   </si>
   <si>
     <t>.time</t>
@@ -1038,10 +1022,10 @@
 </t>
   </si>
   <si>
-    <t>Persons involved in the encounter other than the patient</t>
-  </si>
-  <si>
-    <t>Persons involved in the encounter other than the patient.</t>
+    <t>Persons involved in the timepoint other than the patient</t>
+  </si>
+  <si>
+    <t>Persons involved in the timepoint other than the patient.</t>
   </si>
   <si>
     <t>Event.performer.actor</t>
@@ -1156,7 +1140,7 @@
 </t>
   </si>
   <si>
-    <t>Reason the encounter takes place (reference)</t>
+    <t>Reason the timepoint takes place (reference)</t>
   </si>
   <si>
     <t>Reference Services Provided (Procedure) and/or Reference specific clinical findings (Observation) related to the given timepoint.</t>
@@ -1191,10 +1175,10 @@
 </t>
   </si>
   <si>
-    <t>The diagnosis or procedure relevant to the encounter</t>
-  </si>
-  <si>
-    <t>Reason the encounter takes place, as specified using information from another resource. For admissions, this is the admission diagnosis. The indication will typically be a Condition (with other resources referenced in the evidence.detail), or a Procedure.</t>
+    <t>The diagnosis or procedure relevant to the timepoint</t>
+  </si>
+  <si>
+    <t>Reason the timepoint takes place, as specified using information from another resource. For admissions, this is the admission diagnosis. The indication will typically be a Condition (with other resources referenced in the evidence.detail), or a Procedure.</t>
   </si>
   <si>
     <t>Event.reasonReference</t>
@@ -1209,10 +1193,7 @@
     <t>Encounter.diagnosis.use</t>
   </si>
   <si>
-    <t>Role that this diagnosis has within the encounter (e.g. admission, billing, discharge …)</t>
-  </si>
-  <si>
-    <t>Role that this diagnosis has within the encounter (e.g. admission, billing, discharge …).</t>
+    <t>Role that this diagnosis has within the timepoint (e.g. admission, billing, discharge …)</t>
   </si>
   <si>
     <t>The type of diagnosis this condition represents.</t>
@@ -1244,10 +1225,7 @@
 </t>
   </si>
   <si>
-    <t>The set of accounts that may be used for billing for this Encounter</t>
-  </si>
-  <si>
-    <t>The set of accounts that may be used for billing for this Encounter.</t>
+    <t>The set of accounts that may be used for billing for this timepoint.</t>
   </si>
   <si>
     <t>The billing system may choose to allocate billable items associated with the Encounter to different referenced Accounts based on internal business rules.</t>
@@ -1457,10 +1435,7 @@
     <t>Encounter.location</t>
   </si>
   <si>
-    <t>List of locations where the patient has been</t>
-  </si>
-  <si>
-    <t>List of locations where  the patient has been during this encounter.</t>
+    <t>List of locations where the patient has been during this timepoint.</t>
   </si>
   <si>
     <t>Virtual encounters can be recorded in the Encounter by specifying a location reference to a location of type "kind" such as "client's home" and an encounter.class = "virtual".</t>
@@ -1485,10 +1460,7 @@
 </t>
   </si>
   <si>
-    <t>Location the encounter takes place</t>
-  </si>
-  <si>
-    <t>The location where the encounter takes place.</t>
+    <t>The location where the timepoint takes place.</t>
   </si>
   <si>
     <t>Event.location</t>
@@ -1556,10 +1528,10 @@
 </t>
   </si>
   <si>
-    <t>The organization (facility) responsible for this encounter</t>
-  </si>
-  <si>
-    <t>The organization that is primarily responsible for this Encounter's services. This MAY be the same as the organization on the Patient record, however it could be different, such as if the actor performing the services was from an external organization (which may be billed seperately) for an external consultation.  Refer to the example bundle showing an abbreviated set of Encounters for a colonoscopy.</t>
+    <t>The organization (facility) responsible for this timepoint</t>
+  </si>
+  <si>
+    <t>The organization that is primarily responsible for this timepoint's services. This MAY be the same as the organization on the Patient record, however it could be different, such as if the actor performing the services was from an external organization (which may be billed seperately) for an external consultation. Refer to the example bundle showing an abbreviated set of timepoints for a colonoscopy.</t>
   </si>
   <si>
     <t>.particiaption[typeCode=PFM].role</t>
@@ -1575,10 +1547,7 @@
 </t>
   </si>
   <si>
-    <t>Another Encounter this encounter is part of</t>
-  </si>
-  <si>
-    <t>Another Encounter of which this encounter is a part of (administratively or in time).</t>
+    <t>An Encounter this timepoint is part of</t>
   </si>
   <si>
     <t>This is also used for associating a child's encounter back to the mother's encounter.@@ -1749,7 +1718,7 @@
   <cols>
     <col min="1" max="1" width="45.671875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="12.65625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="63.671875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="3" max="3" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.7734375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.9453125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.4296875" customWidth="true" bestFit="true"/>
@@ -2935,7 +2904,7 @@
         <v>109</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -3001,21 +2970,21 @@
         <v>62</v>
       </c>
       <c r="AJ11" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="AK11" t="s" s="2">
         <v>111</v>
       </c>
-      <c r="AK11" t="s" s="2">
+      <c r="AL11" t="s" s="2">
         <v>112</v>
       </c>
-      <c r="AL11" t="s" s="2">
+      <c r="AM11" t="s" s="2">
         <v>113</v>
-      </c>
-      <c r="AM11" t="s" s="2">
-        <v>114</v>
       </c>
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -3041,10 +3010,10 @@
         <v>52</v>
       </c>
       <c r="K12" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="L12" t="s" s="2">
         <v>116</v>
-      </c>
-      <c r="L12" t="s" s="2">
-        <v>117</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -3095,25 +3064,25 @@
         <v>43</v>
       </c>
       <c r="AE12" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="AF12" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG12" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH12" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI12" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AJ12" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK12" t="s" s="2">
         <v>118</v>
-      </c>
-      <c r="AF12" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG12" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH12" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI12" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AJ12" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK12" t="s" s="2">
-        <v>119</v>
       </c>
       <c r="AL12" t="s" s="2">
         <v>43</v>
@@ -3124,7 +3093,7 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -3153,7 +3122,7 @@
         <v>97</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M13" t="s" s="2">
         <v>99</v>
@@ -3194,19 +3163,19 @@
         <v>43</v>
       </c>
       <c r="AA13" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="AB13" t="s" s="2">
         <v>122</v>
       </c>
-      <c r="AB13" t="s" s="2">
+      <c r="AC13" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD13" t="s" s="2">
         <v>123</v>
       </c>
-      <c r="AC13" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD13" t="s" s="2">
+      <c r="AE13" t="s" s="2">
         <v>124</v>
-      </c>
-      <c r="AE13" t="s" s="2">
-        <v>125</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>41</v>
@@ -3224,7 +3193,7 @@
         <v>43</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL13" t="s" s="2">
         <v>43</v>
@@ -3235,7 +3204,7 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -3261,16 +3230,16 @@
         <v>70</v>
       </c>
       <c r="K14" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="L14" t="s" s="2">
         <v>127</v>
       </c>
-      <c r="L14" t="s" s="2">
+      <c r="M14" t="s" s="2">
         <v>128</v>
       </c>
-      <c r="M14" t="s" s="2">
+      <c r="N14" t="s" s="2">
         <v>129</v>
-      </c>
-      <c r="N14" t="s" s="2">
-        <v>130</v>
       </c>
       <c r="O14" t="s" s="2">
         <v>43</v>
@@ -3295,31 +3264,31 @@
         <v>43</v>
       </c>
       <c r="W14" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="X14" t="s" s="2">
         <v>131</v>
       </c>
-      <c r="X14" t="s" s="2">
+      <c r="Y14" t="s" s="2">
         <v>132</v>
       </c>
-      <c r="Y14" t="s" s="2">
+      <c r="Z14" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA14" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB14" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC14" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD14" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE14" t="s" s="2">
         <v>133</v>
-      </c>
-      <c r="Z14" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA14" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB14" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC14" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD14" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE14" t="s" s="2">
-        <v>134</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>41</v>
@@ -3337,7 +3306,7 @@
         <v>43</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AL14" t="s" s="2">
         <v>43</v>
@@ -3348,7 +3317,7 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -3371,19 +3340,19 @@
         <v>51</v>
       </c>
       <c r="J15" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="K15" t="s" s="2">
         <v>137</v>
       </c>
-      <c r="K15" t="s" s="2">
+      <c r="L15" t="s" s="2">
         <v>138</v>
       </c>
-      <c r="L15" t="s" s="2">
+      <c r="M15" t="s" s="2">
         <v>139</v>
       </c>
-      <c r="M15" t="s" s="2">
+      <c r="N15" t="s" s="2">
         <v>140</v>
-      </c>
-      <c r="N15" t="s" s="2">
-        <v>141</v>
       </c>
       <c r="O15" t="s" s="2">
         <v>43</v>
@@ -3408,31 +3377,31 @@
         <v>43</v>
       </c>
       <c r="W15" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="X15" t="s" s="2">
         <v>142</v>
       </c>
-      <c r="X15" t="s" s="2">
+      <c r="Y15" t="s" s="2">
         <v>143</v>
       </c>
-      <c r="Y15" t="s" s="2">
+      <c r="Z15" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA15" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB15" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC15" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD15" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE15" t="s" s="2">
         <v>144</v>
-      </c>
-      <c r="Z15" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA15" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB15" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC15" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD15" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE15" t="s" s="2">
-        <v>145</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>41</v>
@@ -3450,18 +3419,18 @@
         <v>43</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AL15" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -3487,16 +3456,16 @@
         <v>64</v>
       </c>
       <c r="K16" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="L16" t="s" s="2">
         <v>148</v>
       </c>
-      <c r="L16" t="s" s="2">
+      <c r="M16" t="s" s="2">
         <v>149</v>
       </c>
-      <c r="M16" t="s" s="2">
+      <c r="N16" t="s" s="2">
         <v>150</v>
-      </c>
-      <c r="N16" t="s" s="2">
-        <v>151</v>
       </c>
       <c r="O16" t="s" s="2">
         <v>43</v>
@@ -3509,43 +3478,43 @@
         <v>43</v>
       </c>
       <c r="S16" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="T16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="X16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Y16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE16" t="s" s="2">
         <v>152</v>
-      </c>
-      <c r="T16" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U16" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V16" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W16" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X16" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y16" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z16" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA16" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB16" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC16" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD16" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE16" t="s" s="2">
-        <v>153</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>41</v>
@@ -3563,18 +3532,18 @@
         <v>43</v>
       </c>
       <c r="AK16" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="AL16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM16" t="s" s="2">
         <v>154</v>
-      </c>
-      <c r="AL16" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM16" t="s" s="2">
-        <v>155</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3600,13 +3569,13 @@
         <v>52</v>
       </c>
       <c r="K17" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="L17" t="s" s="2">
         <v>157</v>
       </c>
-      <c r="L17" t="s" s="2">
+      <c r="M17" t="s" s="2">
         <v>158</v>
-      </c>
-      <c r="M17" t="s" s="2">
-        <v>159</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" t="s" s="2">
@@ -3620,43 +3589,43 @@
         <v>43</v>
       </c>
       <c r="S17" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="T17" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U17" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V17" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W17" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="X17" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Y17" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z17" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA17" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB17" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC17" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD17" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE17" t="s" s="2">
         <v>160</v>
-      </c>
-      <c r="T17" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U17" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V17" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W17" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X17" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y17" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z17" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA17" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB17" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC17" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD17" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE17" t="s" s="2">
-        <v>161</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>41</v>
@@ -3674,18 +3643,18 @@
         <v>43</v>
       </c>
       <c r="AK17" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="AL17" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM17" t="s" s="2">
         <v>162</v>
-      </c>
-      <c r="AL17" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM17" t="s" s="2">
-        <v>163</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3708,13 +3677,13 @@
         <v>51</v>
       </c>
       <c r="J18" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="K18" t="s" s="2">
         <v>165</v>
       </c>
-      <c r="K18" t="s" s="2">
+      <c r="L18" t="s" s="2">
         <v>166</v>
-      </c>
-      <c r="L18" t="s" s="2">
-        <v>167</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -3765,7 +3734,7 @@
         <v>43</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>41</v>
@@ -3783,18 +3752,18 @@
         <v>43</v>
       </c>
       <c r="AK18" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="AL18" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM18" t="s" s="2">
         <v>169</v>
-      </c>
-      <c r="AL18" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM18" t="s" s="2">
-        <v>170</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3817,16 +3786,16 @@
         <v>51</v>
       </c>
       <c r="J19" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="K19" t="s" s="2">
         <v>172</v>
       </c>
-      <c r="K19" t="s" s="2">
+      <c r="L19" t="s" s="2">
         <v>173</v>
       </c>
-      <c r="L19" t="s" s="2">
+      <c r="M19" t="s" s="2">
         <v>174</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>175</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
@@ -3876,7 +3845,7 @@
         <v>43</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>41</v>
@@ -3894,18 +3863,18 @@
         <v>43</v>
       </c>
       <c r="AK19" t="s" s="2">
+        <v>176</v>
+      </c>
+      <c r="AL19" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM19" t="s" s="2">
         <v>177</v>
-      </c>
-      <c r="AL19" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM19" t="s" s="2">
-        <v>178</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3931,13 +3900,13 @@
         <v>70</v>
       </c>
       <c r="K20" t="s" s="2">
+        <v>179</v>
+      </c>
+      <c r="L20" t="s" s="2">
+        <v>179</v>
+      </c>
+      <c r="M20" t="s" s="2">
         <v>180</v>
-      </c>
-      <c r="L20" t="s" s="2">
-        <v>181</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>182</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
@@ -3963,13 +3932,11 @@
         <v>43</v>
       </c>
       <c r="W20" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="X20" t="s" s="2">
-        <v>183</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="X20" s="2"/>
       <c r="Y20" t="s" s="2">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="Z20" t="s" s="2">
         <v>43</v>
@@ -3987,7 +3954,7 @@
         <v>43</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>50</v>
@@ -4002,21 +3969,21 @@
         <v>62</v>
       </c>
       <c r="AJ20" t="s" s="2">
+        <v>182</v>
+      </c>
+      <c r="AK20" t="s" s="2">
+        <v>183</v>
+      </c>
+      <c r="AL20" t="s" s="2">
+        <v>184</v>
+      </c>
+      <c r="AM20" t="s" s="2">
         <v>185</v>
-      </c>
-      <c r="AK20" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="AL20" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="AM20" t="s" s="2">
-        <v>188</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -4039,16 +4006,16 @@
         <v>43</v>
       </c>
       <c r="J21" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="K21" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="L21" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="M21" t="s" s="2">
         <v>190</v>
-      </c>
-      <c r="K21" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="L21" t="s" s="2">
-        <v>192</v>
-      </c>
-      <c r="M21" t="s" s="2">
-        <v>193</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
@@ -4098,7 +4065,7 @@
         <v>43</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>41</v>
@@ -4116,7 +4083,7 @@
         <v>43</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL21" t="s" s="2">
         <v>43</v>
@@ -4127,7 +4094,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -4153,10 +4120,10 @@
         <v>52</v>
       </c>
       <c r="K22" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="L22" t="s" s="2">
         <v>116</v>
-      </c>
-      <c r="L22" t="s" s="2">
-        <v>117</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -4207,25 +4174,25 @@
         <v>43</v>
       </c>
       <c r="AE22" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="AF22" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG22" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH22" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI22" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AJ22" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK22" t="s" s="2">
         <v>118</v>
-      </c>
-      <c r="AF22" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG22" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH22" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI22" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AJ22" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK22" t="s" s="2">
-        <v>119</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>43</v>
@@ -4236,7 +4203,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4265,7 +4232,7 @@
         <v>97</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M23" t="s" s="2">
         <v>99</v>
@@ -4318,7 +4285,7 @@
         <v>43</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>41</v>
@@ -4336,7 +4303,7 @@
         <v>43</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>43</v>
@@ -4347,11 +4314,11 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
@@ -4373,10 +4340,10 @@
         <v>96</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="M24" t="s" s="2">
         <v>99</v>
@@ -4431,7 +4398,7 @@
         <v>43</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>41</v>
@@ -4460,7 +4427,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4486,10 +4453,10 @@
         <v>70</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -4516,13 +4483,11 @@
         <v>43</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="X25" t="s" s="2">
-        <v>183</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="X25" s="2"/>
       <c r="Y25" t="s" s="2">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>43</v>
@@ -4540,7 +4505,7 @@
         <v>43</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>50</v>
@@ -4558,7 +4523,7 @@
         <v>43</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>43</v>
@@ -4569,7 +4534,7 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4592,13 +4557,13 @@
         <v>43</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -4649,7 +4614,7 @@
         <v>43</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>50</v>
@@ -4667,7 +4632,7 @@
         <v>43</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL26" t="s" s="2">
         <v>43</v>
@@ -4678,7 +4643,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4701,13 +4666,13 @@
         <v>51</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -4734,13 +4699,13 @@
         <v>43</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>43</v>
@@ -4758,7 +4723,7 @@
         <v>43</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>50</v>
@@ -4776,18 +4741,18 @@
         <v>43</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4810,13 +4775,13 @@
         <v>43</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -4867,7 +4832,7 @@
         <v>43</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>41</v>
@@ -4885,7 +4850,7 @@
         <v>43</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>43</v>
@@ -4896,7 +4861,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4922,10 +4887,10 @@
         <v>52</v>
       </c>
       <c r="K29" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="L29" t="s" s="2">
         <v>116</v>
-      </c>
-      <c r="L29" t="s" s="2">
-        <v>117</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -4976,25 +4941,25 @@
         <v>43</v>
       </c>
       <c r="AE29" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="AF29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG29" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH29" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI29" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AJ29" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK29" t="s" s="2">
         <v>118</v>
-      </c>
-      <c r="AF29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG29" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH29" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI29" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AJ29" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK29" t="s" s="2">
-        <v>119</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>43</v>
@@ -5005,7 +4970,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -5034,7 +4999,7 @@
         <v>97</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M30" t="s" s="2">
         <v>99</v>
@@ -5087,7 +5052,7 @@
         <v>43</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>41</v>
@@ -5105,7 +5070,7 @@
         <v>43</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>43</v>
@@ -5116,11 +5081,11 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
@@ -5142,10 +5107,10 @@
         <v>96</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="M31" t="s" s="2">
         <v>99</v>
@@ -5200,7 +5165,7 @@
         <v>43</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>41</v>
@@ -5229,7 +5194,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5252,13 +5217,13 @@
         <v>43</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -5285,13 +5250,13 @@
         <v>43</v>
       </c>
       <c r="W32" t="s" s="2">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="X32" t="s" s="2">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="Y32" t="s" s="2">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="Z32" t="s" s="2">
         <v>43</v>
@@ -5309,7 +5274,7 @@
         <v>43</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>50</v>
@@ -5327,7 +5292,7 @@
         <v>43</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL32" t="s" s="2">
         <v>43</v>
@@ -5338,7 +5303,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5361,13 +5326,13 @@
         <v>43</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -5418,7 +5383,7 @@
         <v>43</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>50</v>
@@ -5436,7 +5401,7 @@
         <v>43</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL33" t="s" s="2">
         <v>43</v>
@@ -5447,11 +5412,11 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>227</v>
+        <v>43</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
@@ -5470,16 +5435,16 @@
         <v>51</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
@@ -5505,13 +5470,11 @@
         <v>43</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>142</v>
-      </c>
-      <c r="X34" t="s" s="2">
-        <v>231</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="X34" s="2"/>
       <c r="Y34" t="s" s="2">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>43</v>
@@ -5529,7 +5492,7 @@
         <v>43</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>41</v>
@@ -5544,21 +5507,21 @@
         <v>62</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5581,13 +5544,13 @@
         <v>51</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5614,13 +5577,13 @@
         <v>43</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>43</v>
@@ -5638,7 +5601,7 @@
         <v>43</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>41</v>
@@ -5653,21 +5616,21 @@
         <v>62</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5690,13 +5653,13 @@
         <v>43</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5723,13 +5686,13 @@
         <v>43</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="Z36" t="s" s="2">
         <v>43</v>
@@ -5747,7 +5710,7 @@
         <v>43</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>41</v>
@@ -5765,22 +5728,22 @@
         <v>43</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
@@ -5799,16 +5762,16 @@
         <v>51</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
@@ -5858,7 +5821,7 @@
         <v>43</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>41</v>
@@ -5873,21 +5836,21 @@
         <v>62</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5910,13 +5873,13 @@
         <v>51</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5967,7 +5930,7 @@
         <v>43</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>41</v>
@@ -5982,25 +5945,25 @@
         <v>62</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
@@ -6019,13 +5982,13 @@
         <v>43</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -6076,7 +6039,7 @@
         <v>43</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>41</v>
@@ -6091,10 +6054,10 @@
         <v>62</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>43</v>
@@ -6105,7 +6068,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6131,10 +6094,10 @@
         <v>52</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>116</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>117</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -6185,25 +6148,25 @@
         <v>43</v>
       </c>
       <c r="AE40" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="AF40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG40" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH40" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI40" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AJ40" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK40" t="s" s="2">
         <v>118</v>
-      </c>
-      <c r="AF40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG40" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH40" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI40" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AJ40" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK40" t="s" s="2">
-        <v>119</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>43</v>
@@ -6214,7 +6177,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6243,7 +6206,7 @@
         <v>97</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M41" t="s" s="2">
         <v>99</v>
@@ -6284,19 +6247,19 @@
         <v>43</v>
       </c>
       <c r="AA41" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="AB41" t="s" s="2">
         <v>122</v>
       </c>
-      <c r="AB41" t="s" s="2">
+      <c r="AC41" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD41" t="s" s="2">
         <v>123</v>
       </c>
-      <c r="AC41" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD41" t="s" s="2">
+      <c r="AE41" t="s" s="2">
         <v>124</v>
-      </c>
-      <c r="AE41" t="s" s="2">
-        <v>125</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>41</v>
@@ -6314,7 +6277,7 @@
         <v>43</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>43</v>
@@ -6325,10 +6288,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C42" t="s" s="2">
         <v>43</v>
@@ -6350,13 +6313,13 @@
         <v>43</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -6407,7 +6370,7 @@
         <v>43</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>41</v>
@@ -6436,7 +6399,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6462,13 +6425,13 @@
         <v>52</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
@@ -6518,7 +6481,7 @@
         <v>43</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>41</v>
@@ -6527,7 +6490,7 @@
         <v>50</v>
       </c>
       <c r="AH43" t="s" s="2">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="AI43" t="s" s="2">
         <v>62</v>
@@ -6547,7 +6510,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6573,13 +6536,13 @@
         <v>64</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
@@ -6605,13 +6568,13 @@
         <v>43</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="Z44" t="s" s="2">
         <v>43</v>
@@ -6629,7 +6592,7 @@
         <v>43</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>41</v>
@@ -6658,7 +6621,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6684,13 +6647,13 @@
         <v>108</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
@@ -6740,7 +6703,7 @@
         <v>43</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>41</v>
@@ -6758,7 +6721,7 @@
         <v>43</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>43</v>
@@ -6769,7 +6732,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6795,13 +6758,13 @@
         <v>52</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
@@ -6851,7 +6814,7 @@
         <v>43</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>41</v>
@@ -6880,7 +6843,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6903,13 +6866,13 @@
         <v>51</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -6960,7 +6923,7 @@
         <v>43</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>41</v>
@@ -6975,21 +6938,21 @@
         <v>62</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7015,10 +6978,10 @@
         <v>52</v>
       </c>
       <c r="K48" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="L48" t="s" s="2">
         <v>116</v>
-      </c>
-      <c r="L48" t="s" s="2">
-        <v>117</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -7069,25 +7032,25 @@
         <v>43</v>
       </c>
       <c r="AE48" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="AF48" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG48" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH48" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI48" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AJ48" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK48" t="s" s="2">
         <v>118</v>
-      </c>
-      <c r="AF48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG48" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH48" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI48" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AJ48" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK48" t="s" s="2">
-        <v>119</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>43</v>
@@ -7098,7 +7061,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7127,7 +7090,7 @@
         <v>97</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M49" t="s" s="2">
         <v>99</v>
@@ -7180,7 +7143,7 @@
         <v>43</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>41</v>
@@ -7198,7 +7161,7 @@
         <v>43</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>43</v>
@@ -7209,11 +7172,11 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -7235,10 +7198,10 @@
         <v>96</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="M50" t="s" s="2">
         <v>99</v>
@@ -7293,7 +7256,7 @@
         <v>43</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>41</v>
@@ -7322,7 +7285,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7345,16 +7308,16 @@
         <v>51</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
@@ -7380,13 +7343,13 @@
         <v>43</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>43</v>
@@ -7404,7 +7367,7 @@
         <v>43</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>41</v>
@@ -7419,21 +7382,21 @@
         <v>62</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7456,13 +7419,13 @@
         <v>43</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
@@ -7513,7 +7476,7 @@
         <v>43</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>41</v>
@@ -7531,18 +7494,18 @@
         <v>43</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7565,13 +7528,13 @@
         <v>51</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -7622,7 +7585,7 @@
         <v>43</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>41</v>
@@ -7637,21 +7600,21 @@
         <v>62</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7674,13 +7637,13 @@
         <v>51</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -7731,7 +7694,7 @@
         <v>43</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>41</v>
@@ -7746,21 +7709,21 @@
         <v>62</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="AL54" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7783,16 +7746,16 @@
         <v>43</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" t="s" s="2">
@@ -7842,7 +7805,7 @@
         <v>43</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>41</v>
@@ -7857,21 +7820,21 @@
         <v>62</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7894,16 +7857,16 @@
         <v>43</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" t="s" s="2">
@@ -7953,7 +7916,7 @@
         <v>43</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>41</v>
@@ -7968,29 +7931,29 @@
         <v>62</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F57" t="s" s="2">
         <v>42</v>
@@ -8005,16 +7968,16 @@
         <v>51</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" t="s" s="2">
@@ -8043,10 +8006,10 @@
         <v>74</v>
       </c>
       <c r="X57" t="s" s="2">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="Y57" t="s" s="2">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="Z57" t="s" s="2">
         <v>43</v>
@@ -8064,7 +8027,7 @@
         <v>43</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>41</v>
@@ -8079,25 +8042,25 @@
         <v>62</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" t="s" s="2">
@@ -8116,16 +8079,16 @@
         <v>51</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" t="s" s="2">
@@ -8175,7 +8138,7 @@
         <v>43</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>41</v>
@@ -8190,21 +8153,21 @@
         <v>62</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8212,7 +8175,7 @@
       </c>
       <c r="D59" s="2"/>
       <c r="E59" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F59" t="s" s="2">
         <v>42</v>
@@ -8227,13 +8190,13 @@
         <v>51</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -8284,7 +8247,7 @@
         <v>43</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
@@ -8302,7 +8265,7 @@
         <v>43</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>43</v>
@@ -8313,7 +8276,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8339,10 +8302,10 @@
         <v>52</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="L60" t="s" s="2">
         <v>116</v>
-      </c>
-      <c r="L60" t="s" s="2">
-        <v>117</v>
       </c>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
@@ -8393,25 +8356,25 @@
         <v>43</v>
       </c>
       <c r="AE60" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="AF60" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG60" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH60" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI60" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AJ60" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK60" t="s" s="2">
         <v>118</v>
-      </c>
-      <c r="AF60" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG60" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AJ60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK60" t="s" s="2">
-        <v>119</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>43</v>
@@ -8422,7 +8385,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8451,7 +8414,7 @@
         <v>97</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M61" t="s" s="2">
         <v>99</v>
@@ -8504,7 +8467,7 @@
         <v>43</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>41</v>
@@ -8522,7 +8485,7 @@
         <v>43</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL61" t="s" s="2">
         <v>43</v>
@@ -8533,11 +8496,11 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" t="s" s="2">
@@ -8559,10 +8522,10 @@
         <v>96</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="M62" t="s" s="2">
         <v>99</v>
@@ -8617,7 +8580,7 @@
         <v>43</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>41</v>
@@ -8646,11 +8609,11 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" t="s" s="2">
@@ -8669,16 +8632,16 @@
         <v>51</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
@@ -8728,7 +8691,7 @@
         <v>43</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>50</v>
@@ -8743,21 +8706,21 @@
         <v>62</v>
       </c>
       <c r="AJ63" t="s" s="2">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8780,13 +8743,13 @@
         <v>43</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
@@ -8816,10 +8779,10 @@
         <v>74</v>
       </c>
       <c r="X64" t="s" s="2">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="Y64" t="s" s="2">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="Z64" t="s" s="2">
         <v>43</v>
@@ -8837,7 +8800,7 @@
         <v>43</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>41</v>
@@ -8855,7 +8818,7 @@
         <v>43</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL64" t="s" s="2">
         <v>43</v>
@@ -8866,7 +8829,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8889,13 +8852,13 @@
         <v>43</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -8946,7 +8909,7 @@
         <v>43</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>41</v>
@@ -8964,7 +8927,7 @@
         <v>43</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>43</v>
@@ -8975,7 +8938,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8998,16 +8961,16 @@
         <v>43</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
@@ -9057,7 +9020,7 @@
         <v>43</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>41</v>
@@ -9075,7 +9038,7 @@
         <v>43</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="AL66" t="s" s="2">
         <v>43</v>
@@ -9086,7 +9049,7 @@
     </row>
     <row r="67">
       <c r="A67" t="s" s="2">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -9109,16 +9072,16 @@
         <v>43</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="N67" s="2"/>
       <c r="O67" t="s" s="2">
@@ -9168,7 +9131,7 @@
         <v>43</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>41</v>
@@ -9186,7 +9149,7 @@
         <v>43</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="AL67" t="s" s="2">
         <v>43</v>
@@ -9197,7 +9160,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -9223,10 +9186,10 @@
         <v>52</v>
       </c>
       <c r="K68" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="L68" t="s" s="2">
         <v>116</v>
-      </c>
-      <c r="L68" t="s" s="2">
-        <v>117</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
@@ -9277,25 +9240,25 @@
         <v>43</v>
       </c>
       <c r="AE68" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="AF68" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG68" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH68" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI68" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AJ68" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK68" t="s" s="2">
         <v>118</v>
-      </c>
-      <c r="AF68" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG68" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH68" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI68" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AJ68" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK68" t="s" s="2">
-        <v>119</v>
       </c>
       <c r="AL68" t="s" s="2">
         <v>43</v>
@@ -9306,7 +9269,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -9335,7 +9298,7 @@
         <v>97</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M69" t="s" s="2">
         <v>99</v>
@@ -9388,7 +9351,7 @@
         <v>43</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>41</v>
@@ -9406,7 +9369,7 @@
         <v>43</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL69" t="s" s="2">
         <v>43</v>
@@ -9417,11 +9380,11 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" t="s" s="2">
@@ -9443,10 +9406,10 @@
         <v>96</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="M70" t="s" s="2">
         <v>99</v>
@@ -9501,7 +9464,7 @@
         <v>43</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>41</v>
@@ -9530,7 +9493,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9556,10 +9519,10 @@
         <v>108</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -9610,7 +9573,7 @@
         <v>43</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>41</v>
@@ -9628,18 +9591,18 @@
         <v>43</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AL71" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM71" t="s" s="2">
-        <v>409</v>
+        <v>402</v>
       </c>
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9662,13 +9625,13 @@
         <v>43</v>
       </c>
       <c r="J72" t="s" s="2">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
@@ -9719,7 +9682,7 @@
         <v>43</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>41</v>
@@ -9737,7 +9700,7 @@
         <v>43</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="AL72" t="s" s="2">
         <v>43</v>
@@ -9748,7 +9711,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -9771,13 +9734,13 @@
         <v>43</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -9807,10 +9770,10 @@
         <v>74</v>
       </c>
       <c r="X73" t="s" s="2">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="Y73" t="s" s="2">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="Z73" t="s" s="2">
         <v>43</v>
@@ -9828,7 +9791,7 @@
         <v>43</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>41</v>
@@ -9846,18 +9809,18 @@
         <v>43</v>
       </c>
       <c r="AK73" t="s" s="2">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="AL73" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM73" t="s" s="2">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -9880,13 +9843,13 @@
         <v>43</v>
       </c>
       <c r="J74" t="s" s="2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -9913,13 +9876,13 @@
         <v>43</v>
       </c>
       <c r="W74" t="s" s="2">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="X74" t="s" s="2">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="Y74" t="s" s="2">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="Z74" t="s" s="2">
         <v>43</v>
@@ -9937,7 +9900,7 @@
         <v>43</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>41</v>
@@ -9955,18 +9918,18 @@
         <v>43</v>
       </c>
       <c r="AK74" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL74" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM74" t="s" s="2">
-        <v>427</v>
+        <v>420</v>
       </c>
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -9989,19 +9952,19 @@
         <v>43</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="N75" t="s" s="2">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="O75" t="s" s="2">
         <v>43</v>
@@ -10026,13 +9989,13 @@
         <v>43</v>
       </c>
       <c r="W75" t="s" s="2">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="X75" t="s" s="2">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="Y75" t="s" s="2">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="Z75" t="s" s="2">
         <v>43</v>
@@ -10050,7 +10013,7 @@
         <v>43</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>41</v>
@@ -10068,18 +10031,18 @@
         <v>43</v>
       </c>
       <c r="AK75" t="s" s="2">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="AL75" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM75" t="s" s="2">
-        <v>436</v>
+        <v>429</v>
       </c>
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -10102,13 +10065,13 @@
         <v>43</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
@@ -10138,10 +10101,10 @@
         <v>74</v>
       </c>
       <c r="X76" t="s" s="2">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="Y76" t="s" s="2">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="Z76" t="s" s="2">
         <v>43</v>
@@ -10159,7 +10122,7 @@
         <v>43</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>41</v>
@@ -10177,18 +10140,18 @@
         <v>43</v>
       </c>
       <c r="AK76" t="s" s="2">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="AL76" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM76" t="s" s="2">
-        <v>443</v>
+        <v>436</v>
       </c>
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -10211,13 +10174,13 @@
         <v>43</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -10247,10 +10210,10 @@
         <v>74</v>
       </c>
       <c r="X77" t="s" s="2">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="Y77" t="s" s="2">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="Z77" t="s" s="2">
         <v>43</v>
@@ -10268,7 +10231,7 @@
         <v>43</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>41</v>
@@ -10286,18 +10249,18 @@
         <v>43</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="AL77" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM77" t="s" s="2">
-        <v>450</v>
+        <v>443</v>
       </c>
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -10320,13 +10283,13 @@
         <v>43</v>
       </c>
       <c r="J78" t="s" s="2">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -10377,7 +10340,7 @@
         <v>43</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>41</v>
@@ -10395,18 +10358,18 @@
         <v>43</v>
       </c>
       <c r="AK78" t="s" s="2">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="AL78" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM78" t="s" s="2">
-        <v>455</v>
+        <v>448</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s" s="2">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -10429,13 +10392,13 @@
         <v>43</v>
       </c>
       <c r="J79" t="s" s="2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
@@ -10462,13 +10425,13 @@
         <v>43</v>
       </c>
       <c r="W79" t="s" s="2">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="X79" t="s" s="2">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="Y79" t="s" s="2">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="Z79" t="s" s="2">
         <v>43</v>
@@ -10486,7 +10449,7 @@
         <v>43</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>41</v>
@@ -10504,18 +10467,18 @@
         <v>43</v>
       </c>
       <c r="AK79" t="s" s="2">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="AL79" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM79" t="s" s="2">
-        <v>462</v>
+        <v>455</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s" s="2">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10538,16 +10501,16 @@
         <v>43</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="M80" t="s" s="2">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="N80" s="2"/>
       <c r="O80" t="s" s="2">
@@ -10597,7 +10560,7 @@
         <v>43</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>41</v>
@@ -10615,7 +10578,7 @@
         <v>43</v>
       </c>
       <c r="AK80" t="s" s="2">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="AL80" t="s" s="2">
         <v>43</v>
@@ -10626,7 +10589,7 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -10652,10 +10615,10 @@
         <v>52</v>
       </c>
       <c r="K81" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="L81" t="s" s="2">
         <v>116</v>
-      </c>
-      <c r="L81" t="s" s="2">
-        <v>117</v>
       </c>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
@@ -10706,25 +10669,25 @@
         <v>43</v>
       </c>
       <c r="AE81" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="AF81" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG81" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH81" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI81" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AJ81" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK81" t="s" s="2">
         <v>118</v>
-      </c>
-      <c r="AF81" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG81" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AJ81" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK81" t="s" s="2">
-        <v>119</v>
       </c>
       <c r="AL81" t="s" s="2">
         <v>43</v>
@@ -10735,7 +10698,7 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -10764,7 +10727,7 @@
         <v>97</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M82" t="s" s="2">
         <v>99</v>
@@ -10817,7 +10780,7 @@
         <v>43</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AF82" t="s" s="2">
         <v>41</v>
@@ -10835,7 +10798,7 @@
         <v>43</v>
       </c>
       <c r="AK82" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL82" t="s" s="2">
         <v>43</v>
@@ -10846,11 +10809,11 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" t="s" s="2">
@@ -10872,10 +10835,10 @@
         <v>96</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="M83" t="s" s="2">
         <v>99</v>
@@ -10930,7 +10893,7 @@
         <v>43</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>41</v>
@@ -10959,7 +10922,7 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -10982,13 +10945,13 @@
         <v>43</v>
       </c>
       <c r="J84" t="s" s="2">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
@@ -11039,7 +11002,7 @@
         <v>43</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>50</v>
@@ -11054,21 +11017,21 @@
         <v>62</v>
       </c>
       <c r="AJ84" t="s" s="2">
-        <v>475</v>
+        <v>466</v>
       </c>
       <c r="AK84" t="s" s="2">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="AL84" t="s" s="2">
-        <v>476</v>
+        <v>467</v>
       </c>
       <c r="AM84" t="s" s="2">
-        <v>477</v>
+        <v>468</v>
       </c>
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
@@ -11094,13 +11057,13 @@
         <v>70</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="M85" t="s" s="2">
-        <v>481</v>
+        <v>472</v>
       </c>
       <c r="N85" s="2"/>
       <c r="O85" t="s" s="2">
@@ -11126,13 +11089,13 @@
         <v>43</v>
       </c>
       <c r="W85" t="s" s="2">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="X85" t="s" s="2">
-        <v>482</v>
+        <v>473</v>
       </c>
       <c r="Y85" t="s" s="2">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="Z85" t="s" s="2">
         <v>43</v>
@@ -11150,7 +11113,7 @@
         <v>43</v>
       </c>
       <c r="AE85" t="s" s="2">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="AF85" t="s" s="2">
         <v>41</v>
@@ -11168,7 +11131,7 @@
         <v>43</v>
       </c>
       <c r="AK85" t="s" s="2">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="AL85" t="s" s="2">
         <v>43</v>
@@ -11179,7 +11142,7 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
@@ -11202,16 +11165,16 @@
         <v>43</v>
       </c>
       <c r="J86" t="s" s="2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="M86" t="s" s="2">
-        <v>488</v>
+        <v>479</v>
       </c>
       <c r="N86" s="2"/>
       <c r="O86" t="s" s="2">
@@ -11237,13 +11200,13 @@
         <v>43</v>
       </c>
       <c r="W86" t="s" s="2">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="X86" t="s" s="2">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="Y86" t="s" s="2">
-        <v>490</v>
+        <v>481</v>
       </c>
       <c r="Z86" t="s" s="2">
         <v>43</v>
@@ -11261,7 +11224,7 @@
         <v>43</v>
       </c>
       <c r="AE86" t="s" s="2">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="AF86" t="s" s="2">
         <v>41</v>
@@ -11290,7 +11253,7 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" t="s" s="2">
@@ -11313,13 +11276,13 @@
         <v>43</v>
       </c>
       <c r="J87" t="s" s="2">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K87" t="s" s="2">
-        <v>492</v>
+        <v>483</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>493</v>
+        <v>484</v>
       </c>
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
@@ -11370,7 +11333,7 @@
         <v>43</v>
       </c>
       <c r="AE87" t="s" s="2">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="AF87" t="s" s="2">
         <v>41</v>
@@ -11388,7 +11351,7 @@
         <v>43</v>
       </c>
       <c r="AK87" t="s" s="2">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="AL87" t="s" s="2">
         <v>43</v>
@@ -11399,7 +11362,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="2">
-        <v>494</v>
+        <v>485</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" t="s" s="2">
@@ -11422,13 +11385,13 @@
         <v>43</v>
       </c>
       <c r="J88" t="s" s="2">
-        <v>495</v>
+        <v>486</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>496</v>
+        <v>487</v>
       </c>
       <c r="L88" t="s" s="2">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="M88" s="2"/>
       <c r="N88" s="2"/>
@@ -11479,7 +11442,7 @@
         <v>43</v>
       </c>
       <c r="AE88" t="s" s="2">
-        <v>494</v>
+        <v>485</v>
       </c>
       <c r="AF88" t="s" s="2">
         <v>41</v>
@@ -11494,21 +11457,21 @@
         <v>62</v>
       </c>
       <c r="AJ88" t="s" s="2">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="AK88" t="s" s="2">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="AL88" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM88" t="s" s="2">
-        <v>499</v>
+        <v>490</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s" s="2">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" t="s" s="2">
@@ -11531,16 +11494,16 @@
         <v>43</v>
       </c>
       <c r="J89" t="s" s="2">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="K89" t="s" s="2">
-        <v>502</v>
+        <v>493</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>503</v>
+        <v>493</v>
       </c>
       <c r="M89" t="s" s="2">
-        <v>504</v>
+        <v>494</v>
       </c>
       <c r="N89" s="2"/>
       <c r="O89" t="s" s="2">
@@ -11590,7 +11553,7 @@
         <v>43</v>
       </c>
       <c r="AE89" t="s" s="2">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="AF89" t="s" s="2">
         <v>41</v>
@@ -11605,10 +11568,10 @@
         <v>62</v>
       </c>
       <c r="AJ89" t="s" s="2">
-        <v>505</v>
+        <v>495</v>
       </c>
       <c r="AK89" t="s" s="2">
-        <v>506</v>
+        <v>496</v>
       </c>
       <c r="AL89" t="s" s="2">
         <v>43</v>

</xml_diff>

<commit_message>
Add timepoint class code system and value set
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-prat-encounter.xlsx
+++ b/output/StructureDefinition-prat-encounter.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3086" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3084" uniqueCount="495">
   <si>
     <t>Path</t>
   </si>
@@ -659,10 +659,7 @@
     <t>Concepts representing classification of patient timepoint such as ambulatory (outpatient), inpatient, emergency, home health or others due to local variations.</t>
   </si>
   <si>
-    <t>Classification of the encounter.</t>
-  </si>
-  <si>
-    <t>http://terminology.hl7.org/ValueSet/v3-ActEncounterCode</t>
+    <t>http://hl7.org/fhir/us/pacio-rat/ValueSet/prat-class-vs</t>
   </si>
   <si>
     <t>.inboundRelationship[typeCode=SUBJ].source[classCode=LIST].code</t>
@@ -4698,11 +4695,9 @@
       <c r="W27" t="s" s="2">
         <v>141</v>
       </c>
-      <c r="X27" t="s" s="2">
+      <c r="X27" s="2"/>
+      <c r="Y27" t="s" s="2">
         <v>206</v>
-      </c>
-      <c r="Y27" t="s" s="2">
-        <v>207</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>43</v>
@@ -4738,18 +4733,18 @@
         <v>43</v>
       </c>
       <c r="AK27" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="AL27" t="s" s="2">
         <v>208</v>
       </c>
-      <c r="AL27" t="s" s="2">
+      <c r="AM27" t="s" s="2">
         <v>209</v>
-      </c>
-      <c r="AM27" t="s" s="2">
-        <v>210</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4775,10 +4770,10 @@
         <v>187</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="L28" t="s" s="2">
         <v>212</v>
-      </c>
-      <c r="L28" t="s" s="2">
-        <v>213</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -4829,7 +4824,7 @@
         <v>43</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>41</v>
@@ -4858,7 +4853,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4967,7 +4962,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -5078,7 +5073,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5191,7 +5186,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5217,10 +5212,10 @@
         <v>203</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>218</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>219</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -5249,12 +5244,10 @@
       <c r="W32" t="s" s="2">
         <v>141</v>
       </c>
-      <c r="X32" t="s" s="2">
+      <c r="X32" s="2"/>
+      <c r="Y32" t="s" s="2">
         <v>206</v>
       </c>
-      <c r="Y32" t="s" s="2">
-        <v>207</v>
-      </c>
       <c r="Z32" t="s" s="2">
         <v>43</v>
       </c>
@@ -5271,7 +5264,7 @@
         <v>43</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>50</v>
@@ -5300,7 +5293,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5326,10 +5319,10 @@
         <v>164</v>
       </c>
       <c r="K33" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="L33" t="s" s="2">
         <v>221</v>
-      </c>
-      <c r="L33" t="s" s="2">
-        <v>222</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -5380,7 +5373,7 @@
         <v>43</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>50</v>
@@ -5409,7 +5402,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5435,13 +5428,13 @@
         <v>136</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="L34" t="s" s="2">
         <v>224</v>
       </c>
-      <c r="L34" t="s" s="2">
+      <c r="M34" t="s" s="2">
         <v>225</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>226</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
@@ -5471,7 +5464,7 @@
       </c>
       <c r="X34" s="2"/>
       <c r="Y34" t="s" s="2">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>43</v>
@@ -5489,7 +5482,7 @@
         <v>43</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>41</v>
@@ -5504,21 +5497,21 @@
         <v>62</v>
       </c>
       <c r="AJ34" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AK34" t="s" s="2">
         <v>228</v>
       </c>
-      <c r="AK34" t="s" s="2">
+      <c r="AL34" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="AM34" t="s" s="2">
         <v>229</v>
-      </c>
-      <c r="AL34" t="s" s="2">
-        <v>209</v>
-      </c>
-      <c r="AM34" t="s" s="2">
-        <v>230</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5544,10 +5537,10 @@
         <v>136</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>232</v>
-      </c>
-      <c r="L35" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5578,7 +5571,7 @@
       </c>
       <c r="X35" s="2"/>
       <c r="Y35" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>43</v>
@@ -5596,7 +5589,7 @@
         <v>43</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>41</v>
@@ -5611,7 +5604,7 @@
         <v>62</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>118</v>
@@ -5620,12 +5613,12 @@
         <v>43</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5651,10 +5644,10 @@
         <v>136</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5681,14 +5674,14 @@
         <v>43</v>
       </c>
       <c r="W36" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="X36" t="s" s="2">
         <v>238</v>
       </c>
-      <c r="X36" t="s" s="2">
+      <c r="Y36" t="s" s="2">
         <v>239</v>
       </c>
-      <c r="Y36" t="s" s="2">
-        <v>240</v>
-      </c>
       <c r="Z36" t="s" s="2">
         <v>43</v>
       </c>
@@ -5705,7 +5698,7 @@
         <v>43</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>41</v>
@@ -5723,22 +5716,22 @@
         <v>43</v>
       </c>
       <c r="AK36" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="AL36" t="s" s="2">
         <v>241</v>
       </c>
-      <c r="AL36" t="s" s="2">
+      <c r="AM36" t="s" s="2">
         <v>242</v>
-      </c>
-      <c r="AM36" t="s" s="2">
-        <v>243</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
@@ -5757,16 +5750,16 @@
         <v>51</v>
       </c>
       <c r="J37" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="K37" t="s" s="2">
         <v>246</v>
       </c>
-      <c r="K37" t="s" s="2">
+      <c r="L37" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="M37" t="s" s="2">
         <v>247</v>
-      </c>
-      <c r="L37" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>248</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
@@ -5816,7 +5809,7 @@
         <v>43</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>41</v>
@@ -5831,21 +5824,21 @@
         <v>62</v>
       </c>
       <c r="AJ37" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="AK37" t="s" s="2">
         <v>249</v>
       </c>
-      <c r="AK37" t="s" s="2">
+      <c r="AL37" t="s" s="2">
         <v>250</v>
       </c>
-      <c r="AL37" t="s" s="2">
+      <c r="AM37" t="s" s="2">
         <v>251</v>
-      </c>
-      <c r="AM37" t="s" s="2">
-        <v>252</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5868,13 +5861,13 @@
         <v>51</v>
       </c>
       <c r="J38" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="K38" t="s" s="2">
         <v>254</v>
       </c>
-      <c r="K38" t="s" s="2">
+      <c r="L38" t="s" s="2">
         <v>255</v>
-      </c>
-      <c r="L38" t="s" s="2">
-        <v>256</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5925,7 +5918,7 @@
         <v>43</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>41</v>
@@ -5940,25 +5933,25 @@
         <v>62</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>118</v>
       </c>
       <c r="AL38" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="AM38" t="s" s="2">
         <v>258</v>
-      </c>
-      <c r="AM38" t="s" s="2">
-        <v>259</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
@@ -5977,13 +5970,13 @@
         <v>43</v>
       </c>
       <c r="J39" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="K39" t="s" s="2">
         <v>262</v>
       </c>
-      <c r="K39" t="s" s="2">
+      <c r="L39" t="s" s="2">
         <v>263</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>264</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -6034,7 +6027,7 @@
         <v>43</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>41</v>
@@ -6049,10 +6042,10 @@
         <v>62</v>
       </c>
       <c r="AJ39" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="AK39" t="s" s="2">
         <v>265</v>
-      </c>
-      <c r="AK39" t="s" s="2">
-        <v>266</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>43</v>
@@ -6063,7 +6056,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6172,7 +6165,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6283,10 +6276,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="B42" t="s" s="2">
         <v>268</v>
-      </c>
-      <c r="B42" t="s" s="2">
-        <v>269</v>
       </c>
       <c r="C42" t="s" s="2">
         <v>43</v>
@@ -6308,13 +6301,13 @@
         <v>43</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="K42" t="s" s="2">
         <v>270</v>
       </c>
-      <c r="K42" t="s" s="2">
+      <c r="L42" t="s" s="2">
         <v>271</v>
-      </c>
-      <c r="L42" t="s" s="2">
-        <v>272</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -6394,7 +6387,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6420,13 +6413,13 @@
         <v>52</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="L43" t="s" s="2">
         <v>274</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="M43" t="s" s="2">
         <v>275</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>276</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
@@ -6476,16 +6469,16 @@
         <v>43</v>
       </c>
       <c r="AE43" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="AF43" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG43" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH43" t="s" s="2">
         <v>277</v>
-      </c>
-      <c r="AF43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG43" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH43" t="s" s="2">
-        <v>278</v>
       </c>
       <c r="AI43" t="s" s="2">
         <v>62</v>
@@ -6505,7 +6498,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6531,13 +6524,13 @@
         <v>64</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>280</v>
       </c>
-      <c r="L44" t="s" s="2">
+      <c r="M44" t="s" s="2">
         <v>281</v>
-      </c>
-      <c r="M44" t="s" s="2">
-        <v>282</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
@@ -6566,28 +6559,28 @@
         <v>141</v>
       </c>
       <c r="X44" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="Y44" t="s" s="2">
         <v>283</v>
       </c>
-      <c r="Y44" t="s" s="2">
+      <c r="Z44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE44" t="s" s="2">
         <v>284</v>
-      </c>
-      <c r="Z44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE44" t="s" s="2">
-        <v>285</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>41</v>
@@ -6616,7 +6609,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6642,13 +6635,13 @@
         <v>108</v>
       </c>
       <c r="K45" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="L45" t="s" s="2">
         <v>287</v>
       </c>
-      <c r="L45" t="s" s="2">
+      <c r="M45" t="s" s="2">
         <v>288</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>289</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
@@ -6698,7 +6691,7 @@
         <v>43</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>41</v>
@@ -6716,7 +6709,7 @@
         <v>43</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>43</v>
@@ -6727,7 +6720,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6753,13 +6746,13 @@
         <v>52</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="L46" t="s" s="2">
         <v>293</v>
       </c>
-      <c r="L46" t="s" s="2">
+      <c r="M46" t="s" s="2">
         <v>294</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>295</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
@@ -6809,7 +6802,7 @@
         <v>43</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>41</v>
@@ -6838,7 +6831,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6864,10 +6857,10 @@
         <v>187</v>
       </c>
       <c r="K47" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="L47" t="s" s="2">
         <v>298</v>
-      </c>
-      <c r="L47" t="s" s="2">
-        <v>299</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -6918,7 +6911,7 @@
         <v>43</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>41</v>
@@ -6933,21 +6926,21 @@
         <v>62</v>
       </c>
       <c r="AJ47" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="AK47" t="s" s="2">
         <v>300</v>
       </c>
-      <c r="AK47" t="s" s="2">
+      <c r="AL47" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM47" t="s" s="2">
         <v>301</v>
-      </c>
-      <c r="AL47" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM47" t="s" s="2">
-        <v>302</v>
       </c>
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7056,7 +7049,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7167,7 +7160,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7280,7 +7273,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7306,13 +7299,13 @@
         <v>136</v>
       </c>
       <c r="K51" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="L51" t="s" s="2">
         <v>307</v>
       </c>
-      <c r="L51" t="s" s="2">
+      <c r="M51" t="s" s="2">
         <v>308</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>309</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
@@ -7341,11 +7334,11 @@
         <v>141</v>
       </c>
       <c r="X51" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="Y51" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="Y51" t="s" s="2">
-        <v>311</v>
-      </c>
       <c r="Z51" t="s" s="2">
         <v>43</v>
       </c>
@@ -7362,7 +7355,7 @@
         <v>43</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>41</v>
@@ -7377,21 +7370,21 @@
         <v>62</v>
       </c>
       <c r="AJ51" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="AK51" t="s" s="2">
         <v>312</v>
       </c>
-      <c r="AK51" t="s" s="2">
+      <c r="AL51" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM51" t="s" s="2">
         <v>313</v>
-      </c>
-      <c r="AL51" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM51" t="s" s="2">
-        <v>314</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7417,10 +7410,10 @@
         <v>164</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="L52" t="s" s="2">
         <v>316</v>
-      </c>
-      <c r="L52" t="s" s="2">
-        <v>317</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
@@ -7471,7 +7464,7 @@
         <v>43</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>41</v>
@@ -7489,18 +7482,18 @@
         <v>43</v>
       </c>
       <c r="AK52" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="AL52" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM52" t="s" s="2">
         <v>318</v>
-      </c>
-      <c r="AL52" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM52" t="s" s="2">
-        <v>319</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7523,13 +7516,13 @@
         <v>51</v>
       </c>
       <c r="J53" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="K53" t="s" s="2">
         <v>321</v>
       </c>
-      <c r="K53" t="s" s="2">
+      <c r="L53" t="s" s="2">
         <v>322</v>
-      </c>
-      <c r="L53" t="s" s="2">
-        <v>323</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -7580,7 +7573,7 @@
         <v>43</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>41</v>
@@ -7595,21 +7588,21 @@
         <v>62</v>
       </c>
       <c r="AJ53" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="AK53" t="s" s="2">
         <v>324</v>
       </c>
-      <c r="AK53" t="s" s="2">
+      <c r="AL53" t="s" s="2">
         <v>325</v>
       </c>
-      <c r="AL53" t="s" s="2">
+      <c r="AM53" t="s" s="2">
         <v>326</v>
-      </c>
-      <c r="AM53" t="s" s="2">
-        <v>327</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7632,13 +7625,13 @@
         <v>51</v>
       </c>
       <c r="J54" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="K54" t="s" s="2">
         <v>329</v>
       </c>
-      <c r="K54" t="s" s="2">
-        <v>330</v>
-      </c>
       <c r="L54" t="s" s="2">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -7689,7 +7682,7 @@
         <v>43</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>41</v>
@@ -7704,21 +7697,21 @@
         <v>62</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AK54" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="AL54" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM54" t="s" s="2">
         <v>331</v>
-      </c>
-      <c r="AL54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM54" t="s" s="2">
-        <v>332</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7744,13 +7737,13 @@
         <v>164</v>
       </c>
       <c r="K55" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="L55" t="s" s="2">
         <v>334</v>
       </c>
-      <c r="L55" t="s" s="2">
+      <c r="M55" t="s" s="2">
         <v>335</v>
-      </c>
-      <c r="M55" t="s" s="2">
-        <v>336</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" t="s" s="2">
@@ -7800,7 +7793,7 @@
         <v>43</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>41</v>
@@ -7815,21 +7808,21 @@
         <v>62</v>
       </c>
       <c r="AJ55" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="AK55" t="s" s="2">
         <v>337</v>
       </c>
-      <c r="AK55" t="s" s="2">
+      <c r="AL55" t="s" s="2">
         <v>338</v>
       </c>
-      <c r="AL55" t="s" s="2">
+      <c r="AM55" t="s" s="2">
         <v>339</v>
-      </c>
-      <c r="AM55" t="s" s="2">
-        <v>340</v>
       </c>
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7852,16 +7845,16 @@
         <v>43</v>
       </c>
       <c r="J56" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="K56" t="s" s="2">
         <v>342</v>
       </c>
-      <c r="K56" t="s" s="2">
+      <c r="L56" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="M56" t="s" s="2">
         <v>343</v>
-      </c>
-      <c r="L56" t="s" s="2">
-        <v>343</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>344</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" t="s" s="2">
@@ -7911,7 +7904,7 @@
         <v>43</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>41</v>
@@ -7926,25 +7919,25 @@
         <v>62</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AK56" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="AL56" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM56" t="s" s="2">
         <v>345</v>
-      </c>
-      <c r="AL56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM56" t="s" s="2">
-        <v>346</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
@@ -7966,13 +7959,13 @@
         <v>136</v>
       </c>
       <c r="K57" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="L57" t="s" s="2">
         <v>349</v>
       </c>
-      <c r="L57" t="s" s="2">
+      <c r="M57" t="s" s="2">
         <v>350</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>351</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" t="s" s="2">
@@ -8001,11 +7994,11 @@
         <v>74</v>
       </c>
       <c r="X57" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="Y57" t="s" s="2">
         <v>352</v>
       </c>
-      <c r="Y57" t="s" s="2">
-        <v>353</v>
-      </c>
       <c r="Z57" t="s" s="2">
         <v>43</v>
       </c>
@@ -8022,7 +8015,7 @@
         <v>43</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>41</v>
@@ -8037,25 +8030,25 @@
         <v>62</v>
       </c>
       <c r="AJ57" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="AK57" t="s" s="2">
         <v>354</v>
       </c>
-      <c r="AK57" t="s" s="2">
+      <c r="AL57" t="s" s="2">
         <v>355</v>
       </c>
-      <c r="AL57" t="s" s="2">
+      <c r="AM57" t="s" s="2">
         <v>356</v>
-      </c>
-      <c r="AM57" t="s" s="2">
-        <v>357</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" t="s" s="2">
@@ -8074,16 +8067,16 @@
         <v>51</v>
       </c>
       <c r="J58" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="K58" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="K58" t="s" s="2">
+      <c r="L58" t="s" s="2">
         <v>360</v>
       </c>
-      <c r="L58" t="s" s="2">
-        <v>361</v>
-      </c>
       <c r="M58" t="s" s="2">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" t="s" s="2">
@@ -8133,7 +8126,7 @@
         <v>43</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>41</v>
@@ -8148,21 +8141,21 @@
         <v>62</v>
       </c>
       <c r="AJ58" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="AK58" t="s" s="2">
         <v>354</v>
       </c>
-      <c r="AK58" t="s" s="2">
+      <c r="AL58" t="s" s="2">
         <v>355</v>
       </c>
-      <c r="AL58" t="s" s="2">
+      <c r="AM58" t="s" s="2">
         <v>356</v>
-      </c>
-      <c r="AM58" t="s" s="2">
-        <v>357</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8188,10 +8181,10 @@
         <v>187</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -8242,7 +8235,7 @@
         <v>43</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
@@ -8260,7 +8253,7 @@
         <v>43</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>43</v>
@@ -8271,7 +8264,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8380,7 +8373,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8491,7 +8484,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8604,11 +8597,11 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" t="s" s="2">
@@ -8627,16 +8620,16 @@
         <v>51</v>
       </c>
       <c r="J63" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="K63" t="s" s="2">
         <v>370</v>
       </c>
-      <c r="K63" t="s" s="2">
+      <c r="L63" t="s" s="2">
         <v>371</v>
       </c>
-      <c r="L63" t="s" s="2">
-        <v>372</v>
-      </c>
       <c r="M63" t="s" s="2">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
@@ -8686,7 +8679,7 @@
         <v>43</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>50</v>
@@ -8701,21 +8694,21 @@
         <v>62</v>
       </c>
       <c r="AJ63" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="AK63" t="s" s="2">
         <v>373</v>
       </c>
-      <c r="AK63" t="s" s="2">
+      <c r="AL63" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="AM63" t="s" s="2">
         <v>374</v>
-      </c>
-      <c r="AL63" t="s" s="2">
-        <v>356</v>
-      </c>
-      <c r="AM63" t="s" s="2">
-        <v>375</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8741,10 +8734,10 @@
         <v>136</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
@@ -8774,11 +8767,11 @@
         <v>74</v>
       </c>
       <c r="X64" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="Y64" t="s" s="2">
         <v>378</v>
       </c>
-      <c r="Y64" t="s" s="2">
-        <v>379</v>
-      </c>
       <c r="Z64" t="s" s="2">
         <v>43</v>
       </c>
@@ -8795,7 +8788,7 @@
         <v>43</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>41</v>
@@ -8824,7 +8817,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8847,13 +8840,13 @@
         <v>43</v>
       </c>
       <c r="J65" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="K65" t="s" s="2">
         <v>381</v>
       </c>
-      <c r="K65" t="s" s="2">
+      <c r="L65" t="s" s="2">
         <v>382</v>
-      </c>
-      <c r="L65" t="s" s="2">
-        <v>383</v>
       </c>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -8904,7 +8897,7 @@
         <v>43</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>41</v>
@@ -8922,7 +8915,7 @@
         <v>43</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>43</v>
@@ -8933,7 +8926,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8956,16 +8949,16 @@
         <v>43</v>
       </c>
       <c r="J66" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="K66" t="s" s="2">
         <v>386</v>
       </c>
-      <c r="K66" t="s" s="2">
+      <c r="L66" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="M66" t="s" s="2">
         <v>387</v>
-      </c>
-      <c r="L66" t="s" s="2">
-        <v>387</v>
-      </c>
-      <c r="M66" t="s" s="2">
-        <v>388</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
@@ -9015,7 +9008,7 @@
         <v>43</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>41</v>
@@ -9033,7 +9026,7 @@
         <v>43</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AL66" t="s" s="2">
         <v>43</v>
@@ -9044,7 +9037,7 @@
     </row>
     <row r="67">
       <c r="A67" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -9070,13 +9063,13 @@
         <v>187</v>
       </c>
       <c r="K67" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="L67" t="s" s="2">
         <v>391</v>
       </c>
-      <c r="L67" t="s" s="2">
+      <c r="M67" t="s" s="2">
         <v>392</v>
-      </c>
-      <c r="M67" t="s" s="2">
-        <v>393</v>
       </c>
       <c r="N67" s="2"/>
       <c r="O67" t="s" s="2">
@@ -9126,7 +9119,7 @@
         <v>43</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>41</v>
@@ -9144,7 +9137,7 @@
         <v>43</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AL67" t="s" s="2">
         <v>43</v>
@@ -9155,7 +9148,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -9264,7 +9257,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -9375,7 +9368,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -9488,7 +9481,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9514,10 +9507,10 @@
         <v>108</v>
       </c>
       <c r="K71" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="L71" t="s" s="2">
         <v>399</v>
-      </c>
-      <c r="L71" t="s" s="2">
-        <v>400</v>
       </c>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -9568,7 +9561,7 @@
         <v>43</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>41</v>
@@ -9592,12 +9585,12 @@
         <v>43</v>
       </c>
       <c r="AM71" t="s" s="2">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9620,13 +9613,13 @@
         <v>43</v>
       </c>
       <c r="J72" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="K72" t="s" s="2">
         <v>403</v>
       </c>
-      <c r="K72" t="s" s="2">
+      <c r="L72" t="s" s="2">
         <v>404</v>
-      </c>
-      <c r="L72" t="s" s="2">
-        <v>405</v>
       </c>
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
@@ -9677,7 +9670,7 @@
         <v>43</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>41</v>
@@ -9695,7 +9688,7 @@
         <v>43</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="AL72" t="s" s="2">
         <v>43</v>
@@ -9706,7 +9699,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -9732,10 +9725,10 @@
         <v>136</v>
       </c>
       <c r="K73" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="L73" t="s" s="2">
         <v>408</v>
-      </c>
-      <c r="L73" t="s" s="2">
-        <v>409</v>
       </c>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -9765,11 +9758,11 @@
         <v>74</v>
       </c>
       <c r="X73" t="s" s="2">
+        <v>409</v>
+      </c>
+      <c r="Y73" t="s" s="2">
         <v>410</v>
       </c>
-      <c r="Y73" t="s" s="2">
-        <v>411</v>
-      </c>
       <c r="Z73" t="s" s="2">
         <v>43</v>
       </c>
@@ -9786,7 +9779,7 @@
         <v>43</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>41</v>
@@ -9804,18 +9797,18 @@
         <v>43</v>
       </c>
       <c r="AK73" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="AL73" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM73" t="s" s="2">
         <v>412</v>
-      </c>
-      <c r="AL73" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM73" t="s" s="2">
-        <v>413</v>
       </c>
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -9841,10 +9834,10 @@
         <v>136</v>
       </c>
       <c r="K74" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="L74" t="s" s="2">
         <v>415</v>
-      </c>
-      <c r="L74" t="s" s="2">
-        <v>416</v>
       </c>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -9871,14 +9864,14 @@
         <v>43</v>
       </c>
       <c r="W74" t="s" s="2">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X74" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="Y74" t="s" s="2">
         <v>417</v>
       </c>
-      <c r="Y74" t="s" s="2">
-        <v>418</v>
-      </c>
       <c r="Z74" t="s" s="2">
         <v>43</v>
       </c>
@@ -9895,7 +9888,7 @@
         <v>43</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>41</v>
@@ -9919,12 +9912,12 @@
         <v>43</v>
       </c>
       <c r="AM74" t="s" s="2">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -9950,16 +9943,16 @@
         <v>136</v>
       </c>
       <c r="K75" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="L75" t="s" s="2">
         <v>421</v>
       </c>
-      <c r="L75" t="s" s="2">
+      <c r="M75" t="s" s="2">
         <v>422</v>
       </c>
-      <c r="M75" t="s" s="2">
+      <c r="N75" t="s" s="2">
         <v>423</v>
-      </c>
-      <c r="N75" t="s" s="2">
-        <v>424</v>
       </c>
       <c r="O75" t="s" s="2">
         <v>43</v>
@@ -9984,14 +9977,14 @@
         <v>43</v>
       </c>
       <c r="W75" t="s" s="2">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X75" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="Y75" t="s" s="2">
         <v>425</v>
       </c>
-      <c r="Y75" t="s" s="2">
-        <v>426</v>
-      </c>
       <c r="Z75" t="s" s="2">
         <v>43</v>
       </c>
@@ -10008,7 +10001,7 @@
         <v>43</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>41</v>
@@ -10026,18 +10019,18 @@
         <v>43</v>
       </c>
       <c r="AK75" t="s" s="2">
+        <v>426</v>
+      </c>
+      <c r="AL75" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM75" t="s" s="2">
         <v>427</v>
-      </c>
-      <c r="AL75" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM75" t="s" s="2">
-        <v>428</v>
       </c>
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -10063,10 +10056,10 @@
         <v>136</v>
       </c>
       <c r="K76" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="L76" t="s" s="2">
         <v>430</v>
-      </c>
-      <c r="L76" t="s" s="2">
-        <v>431</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
@@ -10096,11 +10089,11 @@
         <v>74</v>
       </c>
       <c r="X76" t="s" s="2">
+        <v>431</v>
+      </c>
+      <c r="Y76" t="s" s="2">
         <v>432</v>
       </c>
-      <c r="Y76" t="s" s="2">
-        <v>433</v>
-      </c>
       <c r="Z76" t="s" s="2">
         <v>43</v>
       </c>
@@ -10117,7 +10110,7 @@
         <v>43</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>41</v>
@@ -10135,18 +10128,18 @@
         <v>43</v>
       </c>
       <c r="AK76" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="AL76" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM76" t="s" s="2">
         <v>434</v>
-      </c>
-      <c r="AL76" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM76" t="s" s="2">
-        <v>435</v>
       </c>
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -10172,10 +10165,10 @@
         <v>136</v>
       </c>
       <c r="K77" t="s" s="2">
+        <v>436</v>
+      </c>
+      <c r="L77" t="s" s="2">
         <v>437</v>
-      </c>
-      <c r="L77" t="s" s="2">
-        <v>438</v>
       </c>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -10205,11 +10198,11 @@
         <v>74</v>
       </c>
       <c r="X77" t="s" s="2">
+        <v>438</v>
+      </c>
+      <c r="Y77" t="s" s="2">
         <v>439</v>
       </c>
-      <c r="Y77" t="s" s="2">
-        <v>440</v>
-      </c>
       <c r="Z77" t="s" s="2">
         <v>43</v>
       </c>
@@ -10226,7 +10219,7 @@
         <v>43</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>41</v>
@@ -10244,18 +10237,18 @@
         <v>43</v>
       </c>
       <c r="AK77" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="AL77" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM77" t="s" s="2">
         <v>441</v>
-      </c>
-      <c r="AL77" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM77" t="s" s="2">
-        <v>442</v>
       </c>
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -10278,13 +10271,13 @@
         <v>43</v>
       </c>
       <c r="J78" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K78" t="s" s="2">
+        <v>443</v>
+      </c>
+      <c r="L78" t="s" s="2">
         <v>444</v>
-      </c>
-      <c r="L78" t="s" s="2">
-        <v>445</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -10335,7 +10328,7 @@
         <v>43</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>41</v>
@@ -10353,18 +10346,18 @@
         <v>43</v>
       </c>
       <c r="AK78" t="s" s="2">
+        <v>445</v>
+      </c>
+      <c r="AL78" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM78" t="s" s="2">
         <v>446</v>
-      </c>
-      <c r="AL78" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM78" t="s" s="2">
-        <v>447</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s" s="2">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -10390,10 +10383,10 @@
         <v>136</v>
       </c>
       <c r="K79" t="s" s="2">
+        <v>448</v>
+      </c>
+      <c r="L79" t="s" s="2">
         <v>449</v>
-      </c>
-      <c r="L79" t="s" s="2">
-        <v>450</v>
       </c>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
@@ -10420,14 +10413,14 @@
         <v>43</v>
       </c>
       <c r="W79" t="s" s="2">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X79" t="s" s="2">
+        <v>450</v>
+      </c>
+      <c r="Y79" t="s" s="2">
         <v>451</v>
       </c>
-      <c r="Y79" t="s" s="2">
-        <v>452</v>
-      </c>
       <c r="Z79" t="s" s="2">
         <v>43</v>
       </c>
@@ -10444,7 +10437,7 @@
         <v>43</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>41</v>
@@ -10462,18 +10455,18 @@
         <v>43</v>
       </c>
       <c r="AK79" t="s" s="2">
+        <v>452</v>
+      </c>
+      <c r="AL79" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM79" t="s" s="2">
         <v>453</v>
-      </c>
-      <c r="AL79" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM79" t="s" s="2">
-        <v>454</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s" s="2">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10499,13 +10492,13 @@
         <v>187</v>
       </c>
       <c r="K80" t="s" s="2">
+        <v>455</v>
+      </c>
+      <c r="L80" t="s" s="2">
+        <v>455</v>
+      </c>
+      <c r="M80" t="s" s="2">
         <v>456</v>
-      </c>
-      <c r="L80" t="s" s="2">
-        <v>456</v>
-      </c>
-      <c r="M80" t="s" s="2">
-        <v>457</v>
       </c>
       <c r="N80" s="2"/>
       <c r="O80" t="s" s="2">
@@ -10555,7 +10548,7 @@
         <v>43</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>41</v>
@@ -10573,7 +10566,7 @@
         <v>43</v>
       </c>
       <c r="AK80" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="AL80" t="s" s="2">
         <v>43</v>
@@ -10584,7 +10577,7 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -10693,7 +10686,7 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -10804,7 +10797,7 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
@@ -10917,7 +10910,7 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -10940,13 +10933,13 @@
         <v>43</v>
       </c>
       <c r="J84" t="s" s="2">
+        <v>462</v>
+      </c>
+      <c r="K84" t="s" s="2">
         <v>463</v>
       </c>
-      <c r="K84" t="s" s="2">
-        <v>464</v>
-      </c>
       <c r="L84" t="s" s="2">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
@@ -10997,7 +10990,7 @@
         <v>43</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>50</v>
@@ -11012,21 +11005,21 @@
         <v>62</v>
       </c>
       <c r="AJ84" t="s" s="2">
+        <v>464</v>
+      </c>
+      <c r="AK84" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="AL84" t="s" s="2">
         <v>465</v>
       </c>
-      <c r="AK84" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="AL84" t="s" s="2">
+      <c r="AM84" t="s" s="2">
         <v>466</v>
-      </c>
-      <c r="AM84" t="s" s="2">
-        <v>467</v>
       </c>
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
@@ -11052,13 +11045,13 @@
         <v>70</v>
       </c>
       <c r="K85" t="s" s="2">
+        <v>468</v>
+      </c>
+      <c r="L85" t="s" s="2">
         <v>469</v>
       </c>
-      <c r="L85" t="s" s="2">
+      <c r="M85" t="s" s="2">
         <v>470</v>
-      </c>
-      <c r="M85" t="s" s="2">
-        <v>471</v>
       </c>
       <c r="N85" s="2"/>
       <c r="O85" t="s" s="2">
@@ -11087,11 +11080,11 @@
         <v>130</v>
       </c>
       <c r="X85" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="Y85" t="s" s="2">
         <v>472</v>
       </c>
-      <c r="Y85" t="s" s="2">
-        <v>473</v>
-      </c>
       <c r="Z85" t="s" s="2">
         <v>43</v>
       </c>
@@ -11108,7 +11101,7 @@
         <v>43</v>
       </c>
       <c r="AE85" t="s" s="2">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="AF85" t="s" s="2">
         <v>41</v>
@@ -11126,7 +11119,7 @@
         <v>43</v>
       </c>
       <c r="AK85" t="s" s="2">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="AL85" t="s" s="2">
         <v>43</v>
@@ -11137,7 +11130,7 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
@@ -11163,13 +11156,13 @@
         <v>136</v>
       </c>
       <c r="K86" t="s" s="2">
+        <v>475</v>
+      </c>
+      <c r="L86" t="s" s="2">
         <v>476</v>
       </c>
-      <c r="L86" t="s" s="2">
+      <c r="M86" t="s" s="2">
         <v>477</v>
-      </c>
-      <c r="M86" t="s" s="2">
-        <v>478</v>
       </c>
       <c r="N86" s="2"/>
       <c r="O86" t="s" s="2">
@@ -11195,14 +11188,14 @@
         <v>43</v>
       </c>
       <c r="W86" t="s" s="2">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X86" t="s" s="2">
+        <v>478</v>
+      </c>
+      <c r="Y86" t="s" s="2">
         <v>479</v>
       </c>
-      <c r="Y86" t="s" s="2">
-        <v>480</v>
-      </c>
       <c r="Z86" t="s" s="2">
         <v>43</v>
       </c>
@@ -11219,7 +11212,7 @@
         <v>43</v>
       </c>
       <c r="AE86" t="s" s="2">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="AF86" t="s" s="2">
         <v>41</v>
@@ -11248,7 +11241,7 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" t="s" s="2">
@@ -11274,10 +11267,10 @@
         <v>164</v>
       </c>
       <c r="K87" t="s" s="2">
+        <v>481</v>
+      </c>
+      <c r="L87" t="s" s="2">
         <v>482</v>
-      </c>
-      <c r="L87" t="s" s="2">
-        <v>483</v>
       </c>
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
@@ -11328,7 +11321,7 @@
         <v>43</v>
       </c>
       <c r="AE87" t="s" s="2">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="AF87" t="s" s="2">
         <v>41</v>
@@ -11346,7 +11339,7 @@
         <v>43</v>
       </c>
       <c r="AK87" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AL87" t="s" s="2">
         <v>43</v>
@@ -11357,7 +11350,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="2">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" t="s" s="2">
@@ -11380,13 +11373,13 @@
         <v>43</v>
       </c>
       <c r="J88" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="K88" t="s" s="2">
         <v>485</v>
       </c>
-      <c r="K88" t="s" s="2">
+      <c r="L88" t="s" s="2">
         <v>486</v>
-      </c>
-      <c r="L88" t="s" s="2">
-        <v>487</v>
       </c>
       <c r="M88" s="2"/>
       <c r="N88" s="2"/>
@@ -11437,7 +11430,7 @@
         <v>43</v>
       </c>
       <c r="AE88" t="s" s="2">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="AF88" t="s" s="2">
         <v>41</v>
@@ -11452,21 +11445,21 @@
         <v>62</v>
       </c>
       <c r="AJ88" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AK88" t="s" s="2">
+        <v>487</v>
+      </c>
+      <c r="AL88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM88" t="s" s="2">
         <v>488</v>
-      </c>
-      <c r="AL88" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM88" t="s" s="2">
-        <v>489</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s" s="2">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" t="s" s="2">
@@ -11489,16 +11482,16 @@
         <v>43</v>
       </c>
       <c r="J89" t="s" s="2">
+        <v>490</v>
+      </c>
+      <c r="K89" t="s" s="2">
         <v>491</v>
       </c>
-      <c r="K89" t="s" s="2">
+      <c r="L89" t="s" s="2">
+        <v>491</v>
+      </c>
+      <c r="M89" t="s" s="2">
         <v>492</v>
-      </c>
-      <c r="L89" t="s" s="2">
-        <v>492</v>
-      </c>
-      <c r="M89" t="s" s="2">
-        <v>493</v>
       </c>
       <c r="N89" s="2"/>
       <c r="O89" t="s" s="2">
@@ -11548,7 +11541,7 @@
         <v>43</v>
       </c>
       <c r="AE89" t="s" s="2">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="AF89" t="s" s="2">
         <v>41</v>
@@ -11563,10 +11556,10 @@
         <v>62</v>
       </c>
       <c r="AJ89" t="s" s="2">
+        <v>493</v>
+      </c>
+      <c r="AK89" t="s" s="2">
         <v>494</v>
-      </c>
-      <c r="AK89" t="s" s="2">
-        <v>495</v>
       </c>
       <c r="AL89" t="s" s="2">
         <v>43</v>

</xml_diff>